<commit_message>
Single file for tables and creating file for each teacher
</commit_message>
<xml_diff>
--- a/PDF to EXCEL/Project/sample.xlsx
+++ b/PDF to EXCEL/Project/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8E661F-5B00-4876-A366-E4809CA13632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4E656-3664-462E-B95A-5D4145E1D2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2134,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999"/>

</xml_diff>